<commit_message>
This is my 14th commit
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shekhar\IdeaProjects\AssignmentFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D44FB1-016D-43A9-A359-295141D54C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1413993E-6FA0-4594-9672-93C763E4B69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Campaigns" sheetId="3" r:id="rId1"/>
     <sheet name="Contacts" sheetId="1" r:id="rId2"/>
     <sheet name="Products" sheetId="4" r:id="rId3"/>
     <sheet name="Login" sheetId="5" r:id="rId4"/>
+    <sheet name="DemoWebLogin" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Organization</t>
   </si>
@@ -72,18 +73,12 @@
     <t>7Vendor_01031 - (Electronics)</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>http://49.249.28.218:8098/</t>
-  </si>
-  <si>
     <t>rmgyantra</t>
   </si>
   <si>
@@ -91,6 +86,15 @@
   </si>
   <si>
     <t>PolycabFan</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>shekuemail@gmail.com</t>
+  </si>
+  <si>
+    <t>$Login123$</t>
   </si>
 </sst>
 </file>
@@ -438,7 +442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C909008-88EA-4978-8FFF-642A196DACDE}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -547,7 +551,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -569,72 +573,71 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43379FB7-7295-4FB8-85DA-F9EDEC0480C4}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{E96E243D-E5BD-40CB-840C-57B0E3691F56}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{6349AE08-399A-4117-9088-B6E68D8166E5}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{B7D55D06-3700-487B-ABD8-B224D0289E9B}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{7EA5057A-8B4D-4F7E-83AF-96D8C0C7099A}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{28D04FDB-934F-4750-91E6-B3E36E4DFE12}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{2B906D42-1AAB-4A97-9351-0344CFA77DE1}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6349AE08-399A-4117-9088-B6E68D8166E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB2159B-DAF3-44FD-908A-A66F4625CEEF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
This is my 16th commit
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shekhar\IdeaProjects\AssignmentFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1413993E-6FA0-4594-9672-93C763E4B69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68C8CB7-C279-4DE2-B8A9-1CC910174E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Campaigns" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
   <si>
     <t>Organization</t>
   </si>
@@ -95,12 +95,187 @@
   </si>
   <si>
     <t>$Login123$</t>
+  </si>
+  <si>
+    <t>abcdef@gmail.com</t>
+  </si>
+  <si>
+    <t>abcdefghijkluoypiio@gmail.com</t>
+  </si>
+  <si>
+    <t>CXzAcC0cA</t>
+  </si>
+  <si>
+    <t>abcdefm</t>
+  </si>
+  <si>
+    <t>abcdefghijkliouyopi@gmail.com</t>
+  </si>
+  <si>
+    <t>CAz0czC1z</t>
+  </si>
+  <si>
+    <t>abcdefghijkliyioupo@gmail.com</t>
+  </si>
+  <si>
+    <t>AXC21XbcX</t>
+  </si>
+  <si>
+    <t>abcdefghijkloiiuypo@gmail.com</t>
+  </si>
+  <si>
+    <t>0b10XX10c</t>
+  </si>
+  <si>
+    <t>abcdefghijklipiuyoo@gmail.com</t>
+  </si>
+  <si>
+    <t>A20XcA0XC</t>
+  </si>
+  <si>
+    <t>abcdefghijkliyuioop@gmail.com</t>
+  </si>
+  <si>
+    <t>A0CAzb1b1</t>
+  </si>
+  <si>
+    <t>abcdefghijkluoipyio@gmail.com</t>
+  </si>
+  <si>
+    <t>b0bc1cbCX</t>
+  </si>
+  <si>
+    <t>abcdefghijkloiyiupo@gmail.com</t>
+  </si>
+  <si>
+    <t>c0A1XCCcb</t>
+  </si>
+  <si>
+    <t>abcdefghijkliioouyp@gmail.com</t>
+  </si>
+  <si>
+    <t>c0bXz0CAC</t>
+  </si>
+  <si>
+    <t>abcdefghijkliiyopuo@gmail.com</t>
+  </si>
+  <si>
+    <t>z01CAC1C0</t>
+  </si>
+  <si>
+    <t>abcdefghijklipioyuo@gmail.com</t>
+  </si>
+  <si>
+    <t>zbCbbz1cc</t>
+  </si>
+  <si>
+    <t>abcdefghijklouiyopi@gmail.com</t>
+  </si>
+  <si>
+    <t>X1c1Ab1c1</t>
+  </si>
+  <si>
+    <t>abcdefghijkliuoioyp@gmail.com</t>
+  </si>
+  <si>
+    <t>zAb2ACXC1</t>
+  </si>
+  <si>
+    <t>abcdefghijkluoiioyp@gmail.com</t>
+  </si>
+  <si>
+    <t>b00AzCz1c</t>
+  </si>
+  <si>
+    <t>abcdefghijklyoiuopi@gmail.com</t>
+  </si>
+  <si>
+    <t>X21A2bcbX</t>
+  </si>
+  <si>
+    <t>abcdefghijklioipyou@gmail.com</t>
+  </si>
+  <si>
+    <t>2zAXz2z2C</t>
+  </si>
+  <si>
+    <t>abcdefghijkluipooiy@gmail.com</t>
+  </si>
+  <si>
+    <t>2cAAzXb2A</t>
+  </si>
+  <si>
+    <t>abcdefghijkluyoiipo@gmail.com</t>
+  </si>
+  <si>
+    <t>zXA2CzACX</t>
+  </si>
+  <si>
+    <t>abcdefghijklouiyiop@gmail.com</t>
+  </si>
+  <si>
+    <t>2A2020zAX</t>
+  </si>
+  <si>
+    <t>abcdefghijklpyuiioo@gmail.com</t>
+  </si>
+  <si>
+    <t>z020XczXc</t>
+  </si>
+  <si>
+    <t>abcdefghijkluoioyip@gmail.com</t>
+  </si>
+  <si>
+    <t>C2220CCb1</t>
+  </si>
+  <si>
+    <t>abcdefghijklyuioiop@gmail.com</t>
+  </si>
+  <si>
+    <t>CbC02b1CA</t>
+  </si>
+  <si>
+    <t>abcdefghijklopiiyuo@gmail.com</t>
+  </si>
+  <si>
+    <t>XA1z2z2c1</t>
+  </si>
+  <si>
+    <t>abcdefghijkliooyupi@gmail.com</t>
+  </si>
+  <si>
+    <t>1CAXXA1AC</t>
+  </si>
+  <si>
+    <t>abcdefghijkluopioiy@gmail.com</t>
+  </si>
+  <si>
+    <t>cc0A1A2c0</t>
+  </si>
+  <si>
+    <t>abcdefghijkloiyoupi@gmail.com</t>
+  </si>
+  <si>
+    <t>bz1z2c2bb</t>
+  </si>
+  <si>
+    <t>abcdefghijkloiuoiyp@gmail.com</t>
+  </si>
+  <si>
+    <t>cXXz01A2z</t>
+  </si>
+  <si>
+    <t>abcdefghijkluyiooip@gmail.com</t>
+  </si>
+  <si>
+    <t>01bXbbccb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,11 +623,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>8</v>
       </c>
     </row>
@@ -476,21 +651,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.77734375"/>
+    <col min="3" max="3" customWidth="true" width="15.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
@@ -509,34 +684,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.88671875"/>
+    <col min="4" max="4" customWidth="true" width="11.6640625"/>
+    <col min="5" max="5" customWidth="true" width="26.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>12</v>
       </c>
       <c r="C2" s="1">
@@ -545,15 +720,15 @@
       <c r="D2" s="1">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>12</v>
       </c>
       <c r="C3" s="1">
@@ -562,7 +737,7 @@
       <c r="D3" s="1">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>13</v>
       </c>
     </row>
@@ -575,14 +750,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43379FB7-7295-4FB8-85DA-F9EDEC0480C4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.33203125"/>
+    <col min="2" max="2" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -613,28 +788,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB2159B-DAF3-44FD-908A-A66F4625CEEF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.21875"/>
+    <col min="2" max="2" customWidth="true" width="11.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>